<commit_message>
Changes for Form PATR
</commit_message>
<xml_diff>
--- a/EvoTax.1099/wwwroot/Templates/Form1099_R_Template.xlsx
+++ b/EvoTax.1099/wwwroot/Templates/Form1099_R_Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://matthewjohnmcnally-my.sharepoint.com/personal/obaig_evolvedtax_com/Documents/Desktop/Excel sample/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Code Repos\EvoTaxes\EvoTax.1099\wwwroot\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="11_A21168594819CF34C8CD04A58E8D08B19E0E7BFC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3ED3FC2-C022-4439-BC45-51D743B0F699}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{891ED841-A817-4B28-B14F-5DCB9ABA745A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="173">
   <si>
     <t>Rcp TIN</t>
   </si>
@@ -536,7 +536,10 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Is Corrected</t>
+    <t>Is Corrected Form of 1099</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -1174,19 +1177,7 @@
     <xf numFmtId="0" fontId="22" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1203,6 +1194,18 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1261,10 +1264,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1533,7 +1532,7 @@
   <dimension ref="A1:AQ13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AQ2" sqref="AQ2:AQ13"/>
+      <selection activeCell="AQ10" sqref="AQ10:AQ13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1911,7 +1910,7 @@
         <v>46</v>
       </c>
       <c r="AQ4" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.35">
@@ -1985,7 +1984,7 @@
         <v>46</v>
       </c>
       <c r="AQ5" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:43" x14ac:dyDescent="0.35">
@@ -2047,7 +2046,7 @@
         <v>46</v>
       </c>
       <c r="AQ6" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:43" x14ac:dyDescent="0.35">
@@ -2118,7 +2117,7 @@
         <v>46</v>
       </c>
       <c r="AQ7" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:43" x14ac:dyDescent="0.35">
@@ -2195,7 +2194,7 @@
         <v>46</v>
       </c>
       <c r="AQ8" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:43" x14ac:dyDescent="0.35">
@@ -2260,7 +2259,7 @@
         <v>46</v>
       </c>
       <c r="AQ9" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:43" x14ac:dyDescent="0.35">
@@ -2556,207 +2555,201 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
       <c r="E1" s="4" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
       <c r="E2" s="5" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
       <c r="E3" s="5" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
       <c r="E4" s="5" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="18"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="23"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="18"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="23"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="14"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A7:K7"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A6:K6"/>
     <mergeCell ref="A15:K15"/>
     <mergeCell ref="A14:K14"/>
     <mergeCell ref="A8:K8"/>
@@ -2765,6 +2758,12 @@
     <mergeCell ref="A11:K11"/>
     <mergeCell ref="A12:K12"/>
     <mergeCell ref="A13:K13"/>
+    <mergeCell ref="A7:K7"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A6:K6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>

</xml_diff>